<commit_message>
write status in excel
</commit_message>
<xml_diff>
--- a/Data/Request.xlsx
+++ b/Data/Request.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\an.m\Documents\UiPath\HelpDeskTicketGeneration\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\an.m\Documents\UiPath\HelpDeskTicketGeneration\Data\Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECDB8E4-E76C-400B-A95E-F94120AD0BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BBC6F0-7178-4CCC-AADB-7C36403331AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="2690" windowWidth="14400" windowHeight="6890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,14 +61,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,7 +83,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,11 +101,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -395,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -406,16 +399,17 @@
     <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -431,7 +425,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C3" s="3"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>